<commit_message>
Cambios finales sprint 1
</commit_message>
<xml_diff>
--- a/docs/sprint 1 - cambios/Sprint 2 Backlog -  Sprint 2 Planning.xlsx
+++ b/docs/sprint 1 - cambios/Sprint 2 Backlog -  Sprint 2 Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caro\Desktop\Sprint1 - cambios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caro\Documents\NetBeansProjects\xtremescrump\docs\sprint 1 - cambios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>Dia 4</t>
   </si>
@@ -239,10 +239,18 @@
     <t>Agregar tareas</t>
   </si>
   <si>
-    <t xml:space="preserve">- </t>
-  </si>
-  <si>
     <t>Calcular esfuerzo de la HU por las tareas</t>
+  </si>
+  <si>
+    <t>-  Se presentará un botón en la columna de Opciones, que diga Agrear tarea.
+- Al hacer clic en el botón se mostrará un diálogo que permite agregar la tarea (Nombre, descripción, esfuerzo), todos los atributos son requeridos.
+- El diálogo tendrá dos botones Guardar y Cancelar. 
+- Al hacer clic en Guardar, se validará que todos los campos requeridos estén llenos, si no es asi se mostrará mensaje de error dando a conocer el campo requerido que no ha sido ingresado.
+- Si la validación ha sido correcta, se guardará la tarea, mostrándose como filas hijas en la tabla de Historia de Usuario.</t>
+  </si>
+  <si>
+    <t>- Al ingresar una tarea el esfuerzo de la Historia de Usuario se calculará por si sólo, siendo la suma de las diferentes tareas.
+- El esfuerzo en la historia de usuario se cambiará a campo no editable.</t>
   </si>
 </sst>
 </file>
@@ -479,6 +487,70 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,93 +593,29 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -893,25 +901,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -927,132 +936,132 @@
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="37" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="44"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,40 +1074,44 @@
       <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-    </row>
-    <row r="16" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="D16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D15:F15"/>
@@ -1115,8 +1128,6 @@
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1125,44 +1136,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A7" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" customWidth="1"/>
-    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1220,188 +1228,188 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
     </row>
     <row r="7" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="40" t="s">
+      <c r="K7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="M7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="40" t="s">
+      <c r="O7" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="53"/>
+      <c r="B8" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="26">
         <v>1</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="28">
         <f xml:space="preserve"> E8</f>
         <v>1</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
     </row>
     <row r="9" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="48" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="26">
         <v>2</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="28">
         <f xml:space="preserve"> E9</f>
         <v>2</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="49" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="18">
         <v>1</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="29">
         <f xml:space="preserve"> E10</f>
         <v>1</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="53" t="s">
+      <c r="A11" s="55"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="18">
         <v>2</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="19">
         <f xml:space="preserve"> E11</f>
         <v>2</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="18">
         <v>1</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="19">
         <f xml:space="preserve"> E12</f>
         <v>1</v>
       </c>
@@ -1416,19 +1424,19 @@
       <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35" t="s">
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="18">
         <v>2</v>
       </c>
-      <c r="F13" s="39">
-        <f t="shared" ref="F13:F21" si="0" xml:space="preserve"> E13</f>
+      <c r="F13" s="19">
+        <f t="shared" ref="F13:F23" si="0" xml:space="preserve"> E13</f>
         <v>2</v>
       </c>
       <c r="G13" s="8"/>
@@ -1442,18 +1450,18 @@
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="18">
         <v>1</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1468,18 +1476,18 @@
       <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="18">
         <v>1</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1494,18 +1502,18 @@
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="18">
         <v>1</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1520,18 +1528,18 @@
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35" t="s">
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="18">
         <v>2</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="19">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1546,70 +1554,70 @@
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="18">
         <v>3</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="19">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="18">
         <v>1</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="18">
         <v>1</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1630,16 +1638,16 @@
       <c r="B21" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="18">
         <v>5</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1653,25 +1661,81 @@
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="32" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-    </row>
-    <row r="24" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-    </row>
-    <row r="25" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="C22" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="18">
+        <v>8</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="18">
+        <v>2</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D26" s="9"/>
@@ -1682,6 +1746,10 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D27" s="9"/>
@@ -1692,6 +1760,10 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="9"/>
@@ -1702,55 +1774,27 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="E29" s="9">
+        <f>SUM(E8:E28)</f>
+        <v>34</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="9"/>
-      <c r="E31" s="9">
-        <f>SUM(E8:E30)</f>
-        <v>24</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="G6:O6"/>
     <mergeCell ref="B12:B20"/>
     <mergeCell ref="A12:A20"/>

</xml_diff>